<commit_message>
New "class" attribute for StyleTag, plus support for CSS files/text.  Use new CellStyleCache and FontCache.  Additional Hyperlink test cases.  Bug fix: adjust borders with merged region in SpanTag.  Bug fix: Recognize "size()" as a collection method and don't perform implicit collections processing.
</commit_message>
<xml_diff>
--- a/jett-core/templates/SpanTagTemplate.xlsx
+++ b/jett-core/templates/SpanTagTemplate.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="375" windowWidth="20715" windowHeight="10485" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="375" windowWidth="20715" windowHeight="10485" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Vert" sheetId="1" r:id="rId1"/>
     <sheet name="Horiz" sheetId="2" r:id="rId2"/>
     <sheet name="VertAdjust" sheetId="3" r:id="rId3"/>
     <sheet name="HorizAdjust" sheetId="4" r:id="rId4"/>
+    <sheet name="VertBorder" sheetId="5" r:id="rId5"/>
+    <sheet name="HorizBorder" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>After1</t>
   </si>
@@ -201,6 +203,18 @@
   </si>
   <si>
     <t>&lt;jt:span adjust="${shrink}" value="Case horiz block adjust=${shrink}" expandRight="true"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:span factor="${expand}" value="factor=${expand}"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:span factor="${expand}" value="factor=${expand}" expandRight="true"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:span adjust="${shrink}" value="adjust=${shrink}"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:span adjust="${shrink}" value="adjust=${shrink}" expandRight="true"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -231,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -239,11 +253,223 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0000FF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF0000FF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0000FF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,6 +486,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1345,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1576,4 +1862,101 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="E2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="E2:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B5:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fix: SpanTag now respects borders by changing the borders to match the new merged region.
</commit_message>
<xml_diff>
--- a/jett-core/templates/SpanTagTemplate.xlsx
+++ b/jett-core/templates/SpanTagTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="375" windowWidth="20715" windowHeight="10485" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="375" windowWidth="20715" windowHeight="10485"/>
   </bookViews>
   <sheets>
     <sheet name="Vert" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>After1</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>&lt;jt:span adjust="${shrink}" value="adjust=${shrink}" expandRight="true"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:span factor="${expand}" value="This is right-justified, which for bug testing purposes doesn't exist anywhere else in the spreadsheet."/&gt;</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -465,11 +468,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -517,6 +557,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,17 +587,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1124,9 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:X7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1866,13 +1914,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>54</v>
       </c>
@@ -1881,33 +1930,45 @@
         <v>56</v>
       </c>
       <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
       <c r="E3" s="13"/>
       <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E4" s="13"/>
       <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E5" s="13"/>
       <c r="F5" s="14"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E6" s="13"/>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="E2:F7"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1923,33 +1984,33 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="18"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Ticket 45 - Bug fix when the color of a Font in a jt:span tag is COLOR_NORMAL (a 32767 value which caused AIOOBE in ExcelColor).
</commit_message>
<xml_diff>
--- a/jett-core/templates/SpanTagTemplate.xlsx
+++ b/jett-core/templates/SpanTagTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="375" windowWidth="20715" windowHeight="10485"/>
+    <workbookView xWindow="600" yWindow="375" windowWidth="20715" windowHeight="10485" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Vert" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="HorizAdjust" sheetId="4" r:id="rId4"/>
     <sheet name="VertBorder" sheetId="5" r:id="rId5"/>
     <sheet name="HorizBorder" sheetId="6" r:id="rId6"/>
+    <sheet name="ColorNormal" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>After1</t>
   </si>
@@ -219,12 +220,15 @@
   <si>
     <t>&lt;jt:span factor="${expand}" value="This is right-justified, which for bug testing purposes doesn't exist anywhere else in the spreadsheet."/&gt;</t>
   </si>
+  <si>
+    <t>&lt;jt:forEach items="${heights}" var="height"&gt;&lt;jt:span factor="${height}" value="${height}"/&gt;&lt;/jt:forEach&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +243,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -248,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -505,11 +515,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,6 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,37 +583,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -597,6 +592,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,7 +931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -913,72 +939,72 @@
       <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -997,72 +1023,72 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1077,72 +1103,72 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1182,211 +1208,211 @@
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
       <c r="P1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
       <c r="X1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
       <c r="P7" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
       <c r="X7" t="s">
         <v>5</v>
       </c>
@@ -1419,72 +1445,72 @@
       <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1503,72 +1529,72 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1583,72 +1609,72 @@
       <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1687,211 +1713,211 @@
       <c r="A1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
       <c r="P1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="Q1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
       <c r="X1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="2"/>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
       <c r="P4" s="2"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
       <c r="P6" s="2"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
       <c r="P7" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
       <c r="X7" t="s">
         <v>5</v>
       </c>
@@ -1922,47 +1948,47 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="9"/>
+      <c r="E2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="H2" s="28" t="s">
+      <c r="F2" s="13"/>
+      <c r="H2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1984,33 +2010,33 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2020,4 +2046,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>